<commit_message>
Changed Trades primary key - ISIN can't be PK for trades
</commit_message>
<xml_diff>
--- a/utils/db-bonds-data.xlsx
+++ b/utils/db-bonds-data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Media_PC\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DB\arrakis_v3\utils\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17A8158B-63F7-4986-B1B3-F1A9217B90BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C9CB4C7-1864-4170-BE09-49B2AFCEDA53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20520" yWindow="2475" windowWidth="20640" windowHeight="11160" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Bonds" sheetId="3" r:id="rId1"/>
@@ -263,6 +263,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd;@"/>
+  </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -760,10 +763,10 @@
   </cellStyleXfs>
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1121,14 +1124,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:J29"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C1048576"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L21" sqref="L21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.44140625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="23.6640625" style="4" customWidth="1"/>
+    <col min="1" max="1" width="24.21875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="23.6640625" style="3" customWidth="1"/>
     <col min="4" max="4" width="19.109375" customWidth="1"/>
     <col min="5" max="5" width="21.6640625" customWidth="1"/>
     <col min="6" max="6" width="14.88671875" customWidth="1"/>
@@ -1137,13 +1140,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B1" t="s">
         <v>15</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="3" t="s">
         <v>76</v>
       </c>
       <c r="D1" t="s">
@@ -1169,16 +1172,16 @@
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B2" t="s">
         <v>23</v>
       </c>
-      <c r="C2" s="4">
+      <c r="C2" s="3">
         <v>1</v>
       </c>
-      <c r="D2" s="1">
+      <c r="D2" s="4">
         <v>44413</v>
       </c>
       <c r="E2">
@@ -1198,16 +1201,16 @@
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B3" t="s">
         <v>23</v>
       </c>
-      <c r="C3" s="4">
+      <c r="C3" s="3">
         <v>1</v>
       </c>
-      <c r="D3" s="1">
+      <c r="D3" s="4">
         <v>44413</v>
       </c>
       <c r="E3">
@@ -1224,16 +1227,16 @@
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="1" t="s">
         <v>28</v>
       </c>
       <c r="B4" t="s">
         <v>23</v>
       </c>
-      <c r="C4" s="4">
+      <c r="C4" s="3">
         <v>2</v>
       </c>
-      <c r="D4" s="1">
+      <c r="D4" s="4">
         <v>44407</v>
       </c>
       <c r="E4">
@@ -1253,16 +1256,16 @@
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="1" t="s">
         <v>28</v>
       </c>
       <c r="B5" t="s">
         <v>23</v>
       </c>
-      <c r="C5" s="4">
+      <c r="C5" s="3">
         <v>2</v>
       </c>
-      <c r="D5" s="1">
+      <c r="D5" s="4">
         <v>44407</v>
       </c>
       <c r="E5">
@@ -1282,16 +1285,16 @@
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="1" t="s">
         <v>33</v>
       </c>
       <c r="B6" t="s">
         <v>23</v>
       </c>
-      <c r="C6" s="4">
+      <c r="C6" s="3">
         <v>3</v>
       </c>
-      <c r="D6" s="1">
+      <c r="D6" s="4">
         <v>44469</v>
       </c>
       <c r="E6">
@@ -1311,16 +1314,16 @@
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="1" t="s">
         <v>28</v>
       </c>
       <c r="B7" t="s">
         <v>23</v>
       </c>
-      <c r="C7" s="4">
+      <c r="C7" s="3">
         <v>2</v>
       </c>
-      <c r="D7" s="1">
+      <c r="D7" s="4">
         <v>44407</v>
       </c>
       <c r="E7">
@@ -1340,16 +1343,16 @@
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="1" t="s">
         <v>33</v>
       </c>
       <c r="B8" t="s">
         <v>23</v>
       </c>
-      <c r="C8" s="4">
+      <c r="C8" s="3">
         <v>3</v>
       </c>
-      <c r="D8" s="1">
+      <c r="D8" s="4">
         <v>44469</v>
       </c>
       <c r="E8">
@@ -1369,16 +1372,16 @@
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A9" s="2" t="s">
+      <c r="A9" s="1" t="s">
         <v>40</v>
       </c>
       <c r="B9" t="s">
         <v>23</v>
       </c>
-      <c r="C9" s="4">
+      <c r="C9" s="3">
         <v>4</v>
       </c>
-      <c r="D9" s="1">
+      <c r="D9" s="4">
         <v>44411</v>
       </c>
       <c r="E9">
@@ -1398,16 +1401,16 @@
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A10" s="2" t="s">
+      <c r="A10" s="1" t="s">
         <v>40</v>
       </c>
       <c r="B10" t="s">
         <v>23</v>
       </c>
-      <c r="C10" s="4">
+      <c r="C10" s="3">
         <v>4</v>
       </c>
-      <c r="D10" s="1">
+      <c r="D10" s="4">
         <v>44411</v>
       </c>
       <c r="E10">
@@ -1427,16 +1430,16 @@
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A11" s="2" t="s">
+      <c r="A11" s="1" t="s">
         <v>45</v>
       </c>
       <c r="B11" t="s">
         <v>47</v>
       </c>
-      <c r="C11" s="4">
+      <c r="C11" s="3">
         <v>5</v>
       </c>
-      <c r="D11" s="1">
+      <c r="D11" s="4">
         <v>44417</v>
       </c>
       <c r="E11">
@@ -1456,16 +1459,16 @@
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A12" s="2" t="s">
+      <c r="A12" s="1" t="s">
         <v>50</v>
       </c>
       <c r="B12" t="s">
         <v>47</v>
       </c>
-      <c r="C12" s="4">
+      <c r="C12" s="3">
         <v>5</v>
       </c>
-      <c r="D12" s="1">
+      <c r="D12" s="4">
         <v>44417</v>
       </c>
       <c r="E12">
@@ -1485,16 +1488,16 @@
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A13" s="2" t="s">
+      <c r="A13" s="1" t="s">
         <v>51</v>
       </c>
       <c r="B13" t="s">
         <v>47</v>
       </c>
-      <c r="C13" s="4">
+      <c r="C13" s="3">
         <v>5</v>
       </c>
-      <c r="D13" s="1">
+      <c r="D13" s="4">
         <v>44417</v>
       </c>
       <c r="E13">
@@ -1514,16 +1517,16 @@
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A14" s="2" t="s">
+      <c r="A14" s="1" t="s">
         <v>53</v>
       </c>
       <c r="B14" t="s">
         <v>47</v>
       </c>
-      <c r="C14" s="4">
+      <c r="C14" s="3">
         <v>5</v>
       </c>
-      <c r="D14" s="1">
+      <c r="D14" s="4">
         <v>44417</v>
       </c>
       <c r="E14">
@@ -1543,16 +1546,16 @@
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A15" s="2" t="s">
+      <c r="A15" s="1" t="s">
         <v>54</v>
       </c>
       <c r="B15" t="s">
         <v>47</v>
       </c>
-      <c r="C15" s="4">
+      <c r="C15" s="3">
         <v>5</v>
       </c>
-      <c r="D15" s="1">
+      <c r="D15" s="4">
         <v>44417</v>
       </c>
       <c r="E15">
@@ -1572,16 +1575,16 @@
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A16" s="2" t="s">
+      <c r="A16" s="1" t="s">
         <v>56</v>
       </c>
       <c r="B16" t="s">
         <v>47</v>
       </c>
-      <c r="C16" s="4">
+      <c r="C16" s="3">
         <v>5</v>
       </c>
-      <c r="D16" s="1">
+      <c r="D16" s="4">
         <v>44417</v>
       </c>
       <c r="E16">
@@ -1601,16 +1604,16 @@
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A17" s="2" t="s">
+      <c r="A17" s="1" t="s">
         <v>57</v>
       </c>
       <c r="B17" t="s">
         <v>47</v>
       </c>
-      <c r="C17" s="4">
+      <c r="C17" s="3">
         <v>5</v>
       </c>
-      <c r="D17" s="1">
+      <c r="D17" s="4">
         <v>44417</v>
       </c>
       <c r="E17">
@@ -1630,16 +1633,16 @@
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A18" s="2" t="s">
+      <c r="A18" s="1" t="s">
         <v>58</v>
       </c>
       <c r="B18" t="s">
         <v>47</v>
       </c>
-      <c r="C18" s="4">
+      <c r="C18" s="3">
         <v>5</v>
       </c>
-      <c r="D18" s="1">
+      <c r="D18" s="4">
         <v>44417</v>
       </c>
       <c r="E18">
@@ -1659,16 +1662,16 @@
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A19" s="2" t="s">
+      <c r="A19" s="1" t="s">
         <v>60</v>
       </c>
       <c r="B19" t="s">
         <v>47</v>
       </c>
-      <c r="C19" s="4">
+      <c r="C19" s="3">
         <v>5</v>
       </c>
-      <c r="D19" s="1">
+      <c r="D19" s="4">
         <v>44417</v>
       </c>
       <c r="E19">
@@ -1688,16 +1691,16 @@
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A20" s="2" t="s">
+      <c r="A20" s="1" t="s">
         <v>62</v>
       </c>
       <c r="B20" t="s">
         <v>47</v>
       </c>
-      <c r="C20" s="4">
+      <c r="C20" s="3">
         <v>5</v>
       </c>
-      <c r="D20" s="1">
+      <c r="D20" s="4">
         <v>44417</v>
       </c>
       <c r="E20">
@@ -1717,16 +1720,16 @@
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A21" s="2" t="s">
+      <c r="A21" s="1" t="s">
         <v>63</v>
       </c>
       <c r="B21" t="s">
         <v>47</v>
       </c>
-      <c r="C21" s="4">
+      <c r="C21" s="3">
         <v>5</v>
       </c>
-      <c r="D21" s="1">
+      <c r="D21" s="4">
         <v>44417</v>
       </c>
       <c r="E21">
@@ -1746,16 +1749,16 @@
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A22" s="2" t="s">
+      <c r="A22" s="1" t="s">
         <v>65</v>
       </c>
       <c r="B22" t="s">
         <v>67</v>
       </c>
-      <c r="C22" s="4">
+      <c r="C22" s="3">
         <v>6</v>
       </c>
-      <c r="D22" s="1">
+      <c r="D22" s="4">
         <v>44414</v>
       </c>
       <c r="E22">
@@ -1775,16 +1778,16 @@
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A23" s="2" t="s">
+      <c r="A23" s="1" t="s">
         <v>65</v>
       </c>
       <c r="B23" t="s">
         <v>67</v>
       </c>
-      <c r="C23" s="4">
+      <c r="C23" s="3">
         <v>6</v>
       </c>
-      <c r="D23" s="1">
+      <c r="D23" s="4">
         <v>44414</v>
       </c>
       <c r="E23">
@@ -1804,16 +1807,16 @@
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A24" s="2" t="s">
+      <c r="A24" s="1" t="s">
         <v>65</v>
       </c>
       <c r="B24" t="s">
         <v>67</v>
       </c>
-      <c r="C24" s="4">
+      <c r="C24" s="3">
         <v>6</v>
       </c>
-      <c r="D24" s="1">
+      <c r="D24" s="4">
         <v>44414</v>
       </c>
       <c r="E24">
@@ -1833,16 +1836,16 @@
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A25" s="2" t="s">
+      <c r="A25" s="1" t="s">
         <v>65</v>
       </c>
       <c r="B25" t="s">
         <v>67</v>
       </c>
-      <c r="C25" s="4">
+      <c r="C25" s="3">
         <v>6</v>
       </c>
-      <c r="D25" s="1">
+      <c r="D25" s="4">
         <v>44414</v>
       </c>
       <c r="E25">
@@ -1862,16 +1865,16 @@
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A26" s="2" t="s">
+      <c r="A26" s="1" t="s">
         <v>69</v>
       </c>
       <c r="B26" t="s">
         <v>67</v>
       </c>
-      <c r="C26" s="4">
+      <c r="C26" s="3">
         <v>7</v>
       </c>
-      <c r="D26" s="1">
+      <c r="D26" s="4">
         <v>47839</v>
       </c>
       <c r="E26">
@@ -1891,16 +1894,16 @@
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A27" s="2" t="s">
+      <c r="A27" s="1" t="s">
         <v>69</v>
       </c>
       <c r="B27" t="s">
         <v>67</v>
       </c>
-      <c r="C27" s="4">
+      <c r="C27" s="3">
         <v>7</v>
       </c>
-      <c r="D27" s="1">
+      <c r="D27" s="4">
         <v>47839</v>
       </c>
       <c r="E27">
@@ -1920,16 +1923,16 @@
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A28" s="2" t="s">
+      <c r="A28" s="1" t="s">
         <v>69</v>
       </c>
       <c r="B28" t="s">
         <v>67</v>
       </c>
-      <c r="C28" s="4">
+      <c r="C28" s="3">
         <v>7</v>
       </c>
-      <c r="D28" s="1">
+      <c r="D28" s="4">
         <v>47839</v>
       </c>
       <c r="E28">
@@ -1949,16 +1952,16 @@
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A29" s="2" t="s">
+      <c r="A29" s="1" t="s">
         <v>69</v>
       </c>
       <c r="B29" t="s">
         <v>67</v>
       </c>
-      <c r="C29" s="4">
+      <c r="C29" s="3">
         <v>7</v>
       </c>
-      <c r="D29" s="1">
+      <c r="D29" s="4">
         <v>47839</v>
       </c>
       <c r="E29">
@@ -1988,15 +1991,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:J29"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="17.44140625" customWidth="1"/>
     <col min="2" max="2" width="16.44140625" customWidth="1"/>
-    <col min="3" max="3" width="21.88671875" style="3" customWidth="1"/>
+    <col min="3" max="3" width="21.88671875" style="2" customWidth="1"/>
     <col min="4" max="4" width="13.5546875" customWidth="1"/>
     <col min="5" max="5" width="13.88671875" customWidth="1"/>
     <col min="6" max="6" width="32.44140625" customWidth="1"/>
@@ -2006,13 +2009,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B1" t="s">
         <v>16</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="2" t="s">
         <v>75</v>
       </c>
       <c r="D1" t="s">
@@ -2038,13 +2041,13 @@
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B2" t="s">
         <v>24</v>
       </c>
-      <c r="C2" s="3">
+      <c r="C2" s="2">
         <v>1</v>
       </c>
       <c r="D2" t="s">
@@ -2059,10 +2062,10 @@
       <c r="G2" t="s">
         <v>17</v>
       </c>
-      <c r="H2" s="1">
+      <c r="H2" s="4">
         <v>44329</v>
       </c>
-      <c r="I2" s="1">
+      <c r="I2" s="4">
         <v>44412</v>
       </c>
       <c r="J2">
@@ -2070,13 +2073,13 @@
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B3" t="s">
         <v>24</v>
       </c>
-      <c r="C3" s="3">
+      <c r="C3" s="2">
         <v>1</v>
       </c>
       <c r="D3" t="s">
@@ -2091,10 +2094,10 @@
       <c r="G3" t="s">
         <v>26</v>
       </c>
-      <c r="H3" s="1">
+      <c r="H3" s="4">
         <v>44231</v>
       </c>
-      <c r="I3" s="1">
+      <c r="I3" s="4">
         <v>44412</v>
       </c>
       <c r="J3">
@@ -2102,13 +2105,13 @@
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="1" t="s">
         <v>28</v>
       </c>
       <c r="B4" t="s">
         <v>30</v>
       </c>
-      <c r="C4" s="3">
+      <c r="C4" s="2">
         <v>2</v>
       </c>
       <c r="D4" t="s">
@@ -2123,10 +2126,10 @@
       <c r="G4" t="s">
         <v>17</v>
       </c>
-      <c r="H4" s="1">
+      <c r="H4" s="4">
         <v>44329</v>
       </c>
-      <c r="I4" s="1">
+      <c r="I4" s="4">
         <v>44431</v>
       </c>
       <c r="J4">
@@ -2134,13 +2137,13 @@
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="1" t="s">
         <v>28</v>
       </c>
       <c r="B5" t="s">
         <v>30</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C5" s="2">
         <v>2</v>
       </c>
       <c r="D5" t="s">
@@ -2155,10 +2158,10 @@
       <c r="G5" t="s">
         <v>26</v>
       </c>
-      <c r="H5" s="1">
+      <c r="H5" s="4">
         <v>44231</v>
       </c>
-      <c r="I5" s="1">
+      <c r="I5" s="4">
         <v>44449</v>
       </c>
       <c r="J5">
@@ -2166,13 +2169,13 @@
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="1" t="s">
         <v>33</v>
       </c>
       <c r="B6" t="s">
         <v>35</v>
       </c>
-      <c r="C6" s="3">
+      <c r="C6" s="2">
         <v>4</v>
       </c>
       <c r="D6" t="s">
@@ -2187,10 +2190,10 @@
       <c r="G6" t="s">
         <v>17</v>
       </c>
-      <c r="H6" s="1">
+      <c r="H6" s="4">
         <v>44329</v>
       </c>
-      <c r="I6" s="1">
+      <c r="I6" s="4">
         <v>44431</v>
       </c>
       <c r="J6">
@@ -2198,13 +2201,13 @@
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="1" t="s">
         <v>28</v>
       </c>
       <c r="B7" t="s">
         <v>30</v>
       </c>
-      <c r="C7" s="3">
+      <c r="C7" s="2">
         <v>3</v>
       </c>
       <c r="D7" t="s">
@@ -2219,10 +2222,10 @@
       <c r="G7" t="s">
         <v>17</v>
       </c>
-      <c r="H7" s="1">
+      <c r="H7" s="4">
         <v>44329</v>
       </c>
-      <c r="I7" s="1">
+      <c r="I7" s="4">
         <v>44431</v>
       </c>
       <c r="J7">
@@ -2230,13 +2233,13 @@
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="1" t="s">
         <v>33</v>
       </c>
       <c r="B8" t="s">
         <v>38</v>
       </c>
-      <c r="C8" s="3">
+      <c r="C8" s="2">
         <v>4</v>
       </c>
       <c r="D8" t="s">
@@ -2251,10 +2254,10 @@
       <c r="G8" t="s">
         <v>26</v>
       </c>
-      <c r="H8" s="1">
+      <c r="H8" s="4">
         <v>44329</v>
       </c>
-      <c r="I8" s="1">
+      <c r="I8" s="4">
         <v>44431</v>
       </c>
       <c r="J8">
@@ -2262,13 +2265,13 @@
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A9" s="2" t="s">
+      <c r="A9" s="1" t="s">
         <v>40</v>
       </c>
       <c r="B9" t="s">
         <v>42</v>
       </c>
-      <c r="C9" s="3">
+      <c r="C9" s="2">
         <v>5</v>
       </c>
       <c r="D9" t="s">
@@ -2283,10 +2286,10 @@
       <c r="G9" t="s">
         <v>17</v>
       </c>
-      <c r="H9" s="1">
+      <c r="H9" s="4">
         <v>44231</v>
       </c>
-      <c r="I9" s="1">
+      <c r="I9" s="4">
         <v>44466</v>
       </c>
       <c r="J9">
@@ -2294,13 +2297,13 @@
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A10" s="2" t="s">
+      <c r="A10" s="1" t="s">
         <v>40</v>
       </c>
       <c r="B10" t="s">
         <v>42</v>
       </c>
-      <c r="C10" s="3">
+      <c r="C10" s="2">
         <v>5</v>
       </c>
       <c r="D10" t="s">
@@ -2315,10 +2318,10 @@
       <c r="G10" t="s">
         <v>17</v>
       </c>
-      <c r="H10" s="1">
+      <c r="H10" s="4">
         <v>44431</v>
       </c>
-      <c r="I10" s="1">
+      <c r="I10" s="4">
         <v>44431</v>
       </c>
       <c r="J10">
@@ -2326,13 +2329,13 @@
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A11" s="2" t="s">
+      <c r="A11" s="1" t="s">
         <v>45</v>
       </c>
       <c r="B11" t="s">
         <v>48</v>
       </c>
-      <c r="C11" s="3">
+      <c r="C11" s="2">
         <v>6</v>
       </c>
       <c r="D11" t="s">
@@ -2347,10 +2350,10 @@
       <c r="G11" t="s">
         <v>17</v>
       </c>
-      <c r="H11" s="1">
+      <c r="H11" s="4">
         <v>44466</v>
       </c>
-      <c r="I11" s="1">
+      <c r="I11" s="4">
         <v>44466</v>
       </c>
       <c r="J11">
@@ -2358,13 +2361,13 @@
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A12" s="2" t="s">
+      <c r="A12" s="1" t="s">
         <v>50</v>
       </c>
       <c r="B12" t="s">
         <v>48</v>
       </c>
-      <c r="C12" s="3">
+      <c r="C12" s="2">
         <v>6</v>
       </c>
       <c r="D12" t="s">
@@ -2379,10 +2382,10 @@
       <c r="G12" t="s">
         <v>26</v>
       </c>
-      <c r="H12" s="1">
+      <c r="H12" s="4">
         <v>44467</v>
       </c>
-      <c r="I12" s="1">
+      <c r="I12" s="4">
         <v>44467</v>
       </c>
       <c r="J12">
@@ -2390,13 +2393,13 @@
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A13" s="2" t="s">
+      <c r="A13" s="1" t="s">
         <v>51</v>
       </c>
       <c r="B13" t="s">
         <v>48</v>
       </c>
-      <c r="C13" s="3">
+      <c r="C13" s="2">
         <v>7</v>
       </c>
       <c r="D13" t="s">
@@ -2411,10 +2414,10 @@
       <c r="G13" t="s">
         <v>17</v>
       </c>
-      <c r="H13" s="1">
+      <c r="H13" s="4">
         <v>44468</v>
       </c>
-      <c r="I13" s="1">
+      <c r="I13" s="4">
         <v>44468</v>
       </c>
       <c r="J13">
@@ -2422,13 +2425,13 @@
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A14" s="2" t="s">
+      <c r="A14" s="1" t="s">
         <v>53</v>
       </c>
       <c r="B14" t="s">
         <v>48</v>
       </c>
-      <c r="C14" s="3">
+      <c r="C14" s="2">
         <v>7</v>
       </c>
       <c r="D14" t="s">
@@ -2443,10 +2446,10 @@
       <c r="G14" t="s">
         <v>26</v>
       </c>
-      <c r="H14" s="1">
+      <c r="H14" s="4">
         <v>44469</v>
       </c>
-      <c r="I14" s="1">
+      <c r="I14" s="4">
         <v>44469</v>
       </c>
       <c r="J14">
@@ -2454,13 +2457,13 @@
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A15" s="2" t="s">
+      <c r="A15" s="1" t="s">
         <v>54</v>
       </c>
       <c r="B15" t="s">
         <v>48</v>
       </c>
-      <c r="C15" s="3">
+      <c r="C15" s="2">
         <v>8</v>
       </c>
       <c r="D15" t="s">
@@ -2475,10 +2478,10 @@
       <c r="G15" t="s">
         <v>17</v>
       </c>
-      <c r="H15" s="1">
+      <c r="H15" s="4">
         <v>44470</v>
       </c>
-      <c r="I15" s="1">
+      <c r="I15" s="4">
         <v>44470</v>
       </c>
       <c r="J15">
@@ -2486,13 +2489,13 @@
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A16" s="2" t="s">
+      <c r="A16" s="1" t="s">
         <v>56</v>
       </c>
       <c r="B16" t="s">
         <v>48</v>
       </c>
-      <c r="C16" s="3">
+      <c r="C16" s="2">
         <v>8</v>
       </c>
       <c r="D16" t="s">
@@ -2507,10 +2510,10 @@
       <c r="G16" t="s">
         <v>17</v>
       </c>
-      <c r="H16" s="1">
+      <c r="H16" s="4">
         <v>43740</v>
       </c>
-      <c r="I16" s="1">
+      <c r="I16" s="4">
         <v>43740</v>
       </c>
       <c r="J16">
@@ -2518,13 +2521,13 @@
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A17" s="2" t="s">
+      <c r="A17" s="1" t="s">
         <v>57</v>
       </c>
       <c r="B17" t="s">
         <v>48</v>
       </c>
-      <c r="C17" s="3">
+      <c r="C17" s="2">
         <v>8</v>
       </c>
       <c r="D17" t="s">
@@ -2539,10 +2542,10 @@
       <c r="G17" t="s">
         <v>26</v>
       </c>
-      <c r="H17" s="1">
+      <c r="H17" s="4">
         <v>43741</v>
       </c>
-      <c r="I17" s="1">
+      <c r="I17" s="4">
         <v>43741</v>
       </c>
       <c r="J17">
@@ -2550,13 +2553,13 @@
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A18" s="2" t="s">
+      <c r="A18" s="1" t="s">
         <v>58</v>
       </c>
       <c r="B18" t="s">
         <v>48</v>
       </c>
-      <c r="C18" s="3">
+      <c r="C18" s="2">
         <v>9</v>
       </c>
       <c r="D18" t="s">
@@ -2571,10 +2574,10 @@
       <c r="G18" t="s">
         <v>17</v>
       </c>
-      <c r="H18" s="1">
+      <c r="H18" s="4">
         <v>43377</v>
       </c>
-      <c r="I18" s="1">
+      <c r="I18" s="4">
         <v>43377</v>
       </c>
       <c r="J18">
@@ -2582,13 +2585,13 @@
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A19" s="2" t="s">
+      <c r="A19" s="1" t="s">
         <v>60</v>
       </c>
       <c r="B19" t="s">
         <v>48</v>
       </c>
-      <c r="C19" s="3">
+      <c r="C19" s="2">
         <v>10</v>
       </c>
       <c r="D19" t="s">
@@ -2603,10 +2606,10 @@
       <c r="G19" t="s">
         <v>17</v>
       </c>
-      <c r="H19" s="1">
+      <c r="H19" s="4">
         <v>43743</v>
       </c>
-      <c r="I19" s="1">
+      <c r="I19" s="4">
         <v>43743</v>
       </c>
       <c r="J19">
@@ -2614,13 +2617,13 @@
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A20" s="2" t="s">
+      <c r="A20" s="1" t="s">
         <v>62</v>
       </c>
       <c r="B20" t="s">
         <v>48</v>
       </c>
-      <c r="C20" s="3">
+      <c r="C20" s="2">
         <v>10</v>
       </c>
       <c r="D20" t="s">
@@ -2635,10 +2638,10 @@
       <c r="G20" t="s">
         <v>17</v>
       </c>
-      <c r="H20" s="1">
+      <c r="H20" s="4">
         <v>44353</v>
       </c>
-      <c r="I20" s="1">
+      <c r="I20" s="4">
         <v>44353</v>
       </c>
       <c r="J20">
@@ -2646,13 +2649,13 @@
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A21" s="2" t="s">
+      <c r="A21" s="1" t="s">
         <v>63</v>
       </c>
       <c r="B21" t="s">
         <v>48</v>
       </c>
-      <c r="C21" s="3">
+      <c r="C21" s="2">
         <v>10</v>
       </c>
       <c r="D21" t="s">
@@ -2667,10 +2670,10 @@
       <c r="G21" t="s">
         <v>26</v>
       </c>
-      <c r="H21" s="1">
+      <c r="H21" s="4">
         <v>40823</v>
       </c>
-      <c r="I21" s="1">
+      <c r="I21" s="4">
         <v>44476</v>
       </c>
       <c r="J21">
@@ -2678,13 +2681,13 @@
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A22" s="2" t="s">
+      <c r="A22" s="1" t="s">
         <v>65</v>
       </c>
       <c r="B22" t="s">
         <v>42</v>
       </c>
-      <c r="C22" s="3">
+      <c r="C22" s="2">
         <v>11</v>
       </c>
       <c r="D22" t="s">
@@ -2699,10 +2702,10 @@
       <c r="G22" t="s">
         <v>17</v>
       </c>
-      <c r="H22" s="1">
+      <c r="H22" s="4">
         <v>40943</v>
       </c>
-      <c r="I22" s="1">
+      <c r="I22" s="4">
         <v>44466</v>
       </c>
       <c r="J22">
@@ -2710,13 +2713,13 @@
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A23" s="2" t="s">
+      <c r="A23" s="1" t="s">
         <v>65</v>
       </c>
       <c r="B23" t="s">
         <v>42</v>
       </c>
-      <c r="C23" s="3">
+      <c r="C23" s="2">
         <v>11</v>
       </c>
       <c r="D23" t="s">
@@ -2731,10 +2734,10 @@
       <c r="G23" t="s">
         <v>17</v>
       </c>
-      <c r="H23" s="1">
+      <c r="H23" s="4">
         <v>41144</v>
       </c>
-      <c r="I23" s="1">
+      <c r="I23" s="4">
         <v>44431</v>
       </c>
       <c r="J23">
@@ -2742,13 +2745,13 @@
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A24" s="2" t="s">
+      <c r="A24" s="1" t="s">
         <v>65</v>
       </c>
       <c r="B24" t="s">
         <v>42</v>
       </c>
-      <c r="C24" s="3">
+      <c r="C24" s="2">
         <v>11</v>
       </c>
       <c r="D24" t="s">
@@ -2763,10 +2766,10 @@
       <c r="G24" t="s">
         <v>17</v>
       </c>
-      <c r="H24" s="1">
+      <c r="H24" s="4">
         <v>41309</v>
       </c>
-      <c r="I24" s="1">
+      <c r="I24" s="4">
         <v>44466</v>
       </c>
       <c r="J24">
@@ -2774,13 +2777,13 @@
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A25" s="2" t="s">
+      <c r="A25" s="1" t="s">
         <v>65</v>
       </c>
       <c r="B25" t="s">
         <v>42</v>
       </c>
-      <c r="C25" s="3">
+      <c r="C25" s="2">
         <v>11</v>
       </c>
       <c r="D25" t="s">
@@ -2795,10 +2798,10 @@
       <c r="G25" t="s">
         <v>17</v>
       </c>
-      <c r="H25" s="1">
+      <c r="H25" s="4">
         <v>41874</v>
       </c>
-      <c r="I25" s="1">
+      <c r="I25" s="4">
         <v>44431</v>
       </c>
       <c r="J25">
@@ -2806,13 +2809,13 @@
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A26" s="2" t="s">
+      <c r="A26" s="1" t="s">
         <v>69</v>
       </c>
       <c r="B26" t="s">
         <v>42</v>
       </c>
-      <c r="C26" s="3">
+      <c r="C26" s="2">
         <v>11</v>
       </c>
       <c r="D26" t="s">
@@ -2827,10 +2830,10 @@
       <c r="G26" t="s">
         <v>17</v>
       </c>
-      <c r="H26" s="1">
+      <c r="H26" s="4">
         <v>42404</v>
       </c>
-      <c r="I26" s="1">
+      <c r="I26" s="4">
         <v>44466</v>
       </c>
       <c r="J26">
@@ -2838,13 +2841,13 @@
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A27" s="2" t="s">
+      <c r="A27" s="1" t="s">
         <v>69</v>
       </c>
       <c r="B27" t="s">
         <v>42</v>
       </c>
-      <c r="C27" s="3">
+      <c r="C27" s="2">
         <v>11</v>
       </c>
       <c r="D27" t="s">
@@ -2859,10 +2862,10 @@
       <c r="G27" t="s">
         <v>17</v>
       </c>
-      <c r="H27" s="1">
+      <c r="H27" s="4">
         <v>41144</v>
       </c>
-      <c r="I27" s="1">
+      <c r="I27" s="4">
         <v>44431</v>
       </c>
       <c r="J27">
@@ -2870,13 +2873,13 @@
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A28" s="2" t="s">
+      <c r="A28" s="1" t="s">
         <v>69</v>
       </c>
       <c r="B28" t="s">
         <v>42</v>
       </c>
-      <c r="C28" s="3">
+      <c r="C28" s="2">
         <v>11</v>
       </c>
       <c r="D28" t="s">
@@ -2891,10 +2894,10 @@
       <c r="G28" t="s">
         <v>17</v>
       </c>
-      <c r="H28" s="1">
+      <c r="H28" s="4">
         <v>41309</v>
       </c>
-      <c r="I28" s="1">
+      <c r="I28" s="4">
         <v>44466</v>
       </c>
       <c r="J28">
@@ -2902,13 +2905,13 @@
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A29" s="2" t="s">
+      <c r="A29" s="1" t="s">
         <v>69</v>
       </c>
       <c r="B29" t="s">
         <v>42</v>
       </c>
-      <c r="C29" s="3">
+      <c r="C29" s="2">
         <v>11</v>
       </c>
       <c r="D29" t="s">
@@ -2923,10 +2926,10 @@
       <c r="G29" t="s">
         <v>26</v>
       </c>
-      <c r="H29" s="1">
+      <c r="H29" s="4">
         <v>42239</v>
       </c>
-      <c r="I29" s="1">
+      <c r="I29" s="4">
         <v>44431</v>
       </c>
       <c r="J29">
@@ -2943,18 +2946,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F92B6539-D5A2-42D1-A24A-A879A9B57698}">
   <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" style="3"/>
+    <col min="1" max="1" width="8.88671875" style="2"/>
     <col min="2" max="2" width="21.88671875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="2" t="s">
         <v>73</v>
       </c>
       <c r="B1" t="s">
@@ -2962,7 +2963,7 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" s="3">
+      <c r="A2" s="2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
@@ -2970,7 +2971,7 @@
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" s="3">
+      <c r="A3" s="2">
         <v>2</v>
       </c>
       <c r="B3" t="s">
@@ -2978,7 +2979,7 @@
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" s="3">
+      <c r="A4" s="2">
         <v>3</v>
       </c>
       <c r="B4" t="s">
@@ -2986,7 +2987,7 @@
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" s="3">
+      <c r="A5" s="2">
         <v>4</v>
       </c>
       <c r="B5" t="s">
@@ -2994,7 +2995,7 @@
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" s="3">
+      <c r="A6" s="2">
         <v>5</v>
       </c>
       <c r="B6" t="s">
@@ -3002,7 +3003,7 @@
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" s="3">
+      <c r="A7" s="2">
         <v>6</v>
       </c>
       <c r="B7" t="s">
@@ -3010,7 +3011,7 @@
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A8" s="3">
+      <c r="A8" s="2">
         <v>7</v>
       </c>
       <c r="B8" t="s">
@@ -3018,7 +3019,7 @@
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A9" s="3">
+      <c r="A9" s="2">
         <v>8</v>
       </c>
       <c r="B9" t="s">
@@ -3026,7 +3027,7 @@
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A10" s="3">
+      <c r="A10" s="2">
         <v>9</v>
       </c>
       <c r="B10" t="s">
@@ -3034,7 +3035,7 @@
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A11" s="3">
+      <c r="A11" s="2">
         <v>10</v>
       </c>
       <c r="B11" t="s">
@@ -3042,7 +3043,7 @@
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A12" s="3">
+      <c r="A12" s="2">
         <v>11</v>
       </c>
       <c r="B12" t="s">
@@ -3058,18 +3059,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD1EBF2C-B60E-45F3-B641-72B1A1E58AE6}">
   <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" style="4"/>
+    <col min="1" max="1" width="8.88671875" style="3"/>
     <col min="2" max="2" width="23.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="3" t="s">
         <v>73</v>
       </c>
       <c r="B1" t="s">
@@ -3077,7 +3078,7 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" s="4">
+      <c r="A2" s="3">
         <v>1</v>
       </c>
       <c r="B2" t="s">
@@ -3085,7 +3086,7 @@
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" s="4">
+      <c r="A3" s="3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
@@ -3093,7 +3094,7 @@
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" s="4">
+      <c r="A4" s="3">
         <v>3</v>
       </c>
       <c r="B4" t="s">
@@ -3101,7 +3102,7 @@
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" s="4">
+      <c r="A5" s="3">
         <v>4</v>
       </c>
       <c r="B5" t="s">
@@ -3109,7 +3110,7 @@
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" s="4">
+      <c r="A6" s="3">
         <v>5</v>
       </c>
       <c r="B6" t="s">
@@ -3117,7 +3118,7 @@
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" s="4">
+      <c r="A7" s="3">
         <v>6</v>
       </c>
       <c r="B7" t="s">
@@ -3125,7 +3126,7 @@
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A8" s="4">
+      <c r="A8" s="3">
         <v>7</v>
       </c>
       <c r="B8" t="s">

</xml_diff>

<commit_message>
Removed duplicates of bonds from xlsx file
</commit_message>
<xml_diff>
--- a/utils/db-bonds-data.xlsx
+++ b/utils/db-bonds-data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DB\arrakis_v3\utils\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C9CB4C7-1864-4170-BE09-49B2AFCEDA53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8470402-2994-4F48-B63B-5A7C9225F91F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Bonds" sheetId="3" r:id="rId1"/>
@@ -19,14 +19,14 @@
     <sheet name="Bonds Counter Parties" sheetId="5" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Bonds!$A$1:$J$29</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Bonds!$A$1:$J$8</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="77">
   <si>
     <t>trade_type</t>
   </si>
@@ -264,7 +264,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd;@"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
@@ -766,7 +766,7 @@
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1122,10 +1122,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:J29"/>
+  <dimension ref="A1:J8"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L21" sqref="L21"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1202,42 +1202,45 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="B3" t="s">
         <v>23</v>
       </c>
       <c r="C3" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D3" s="4">
-        <v>44413</v>
+        <v>44407</v>
       </c>
       <c r="E3">
-        <v>1000</v>
+        <v>900</v>
       </c>
       <c r="F3" t="s">
         <v>18</v>
       </c>
       <c r="G3">
-        <v>4.37</v>
+        <v>3.15</v>
       </c>
       <c r="H3" t="s">
         <v>22</v>
       </c>
+      <c r="I3">
+        <v>123456780</v>
+      </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="B4" t="s">
         <v>23</v>
       </c>
       <c r="C4" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D4" s="4">
-        <v>44407</v>
+        <v>44469</v>
       </c>
       <c r="E4">
         <v>900</v>
@@ -1246,27 +1249,27 @@
         <v>18</v>
       </c>
       <c r="G4">
-        <v>3.15</v>
+        <v>2</v>
       </c>
       <c r="H4" t="s">
         <v>22</v>
       </c>
-      <c r="I4">
-        <v>123456780</v>
+      <c r="I4" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>28</v>
+        <v>40</v>
       </c>
       <c r="B5" t="s">
         <v>23</v>
       </c>
       <c r="C5" s="3">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D5" s="4">
-        <v>44407</v>
+        <v>44411</v>
       </c>
       <c r="E5">
         <v>900</v>
@@ -1280,708 +1283,99 @@
       <c r="H5" t="s">
         <v>22</v>
       </c>
-      <c r="I5">
-        <v>123456780</v>
+      <c r="I5" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>33</v>
+        <v>63</v>
       </c>
       <c r="B6" t="s">
-        <v>23</v>
+        <v>47</v>
       </c>
       <c r="C6" s="3">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D6" s="4">
-        <v>44469</v>
+        <v>44417</v>
       </c>
       <c r="E6">
         <v>900</v>
       </c>
       <c r="F6" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="G6">
-        <v>2</v>
+        <v>0.75</v>
       </c>
       <c r="H6" t="s">
         <v>22</v>
       </c>
       <c r="I6" t="s">
-        <v>32</v>
+        <v>44</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>28</v>
+        <v>65</v>
       </c>
       <c r="B7" t="s">
-        <v>23</v>
+        <v>67</v>
       </c>
       <c r="C7" s="3">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="D7" s="4">
-        <v>44407</v>
+        <v>44414</v>
       </c>
       <c r="E7">
-        <v>900</v>
+        <v>690</v>
       </c>
       <c r="F7" t="s">
         <v>18</v>
       </c>
       <c r="G7">
-        <v>3.15</v>
+        <v>2.02</v>
       </c>
       <c r="H7" t="s">
         <v>22</v>
       </c>
-      <c r="I7">
-        <v>123456780</v>
+      <c r="I7" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>33</v>
+        <v>69</v>
       </c>
       <c r="B8" t="s">
-        <v>23</v>
+        <v>67</v>
       </c>
       <c r="C8" s="3">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="D8" s="4">
-        <v>44469</v>
+        <v>47839</v>
       </c>
       <c r="E8">
-        <v>900</v>
+        <v>340</v>
       </c>
       <c r="F8" t="s">
         <v>18</v>
       </c>
       <c r="G8">
-        <v>2</v>
+        <v>1.123</v>
       </c>
       <c r="H8" t="s">
         <v>22</v>
       </c>
       <c r="I8" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A9" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="B9" t="s">
-        <v>23</v>
-      </c>
-      <c r="C9" s="3">
-        <v>4</v>
-      </c>
-      <c r="D9" s="4">
-        <v>44411</v>
-      </c>
-      <c r="E9">
-        <v>900</v>
-      </c>
-      <c r="F9" t="s">
-        <v>18</v>
-      </c>
-      <c r="G9">
-        <v>3.15</v>
-      </c>
-      <c r="H9" t="s">
-        <v>22</v>
-      </c>
-      <c r="I9" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A10" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="B10" t="s">
-        <v>23</v>
-      </c>
-      <c r="C10" s="3">
-        <v>4</v>
-      </c>
-      <c r="D10" s="4">
-        <v>44411</v>
-      </c>
-      <c r="E10">
-        <v>900</v>
-      </c>
-      <c r="F10" t="s">
-        <v>18</v>
-      </c>
-      <c r="G10">
-        <v>3.15</v>
-      </c>
-      <c r="H10" t="s">
-        <v>22</v>
-      </c>
-      <c r="I10" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A11" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="B11" t="s">
-        <v>47</v>
-      </c>
-      <c r="C11" s="3">
-        <v>5</v>
-      </c>
-      <c r="D11" s="4">
-        <v>44417</v>
-      </c>
-      <c r="E11">
-        <v>900</v>
-      </c>
-      <c r="F11" t="s">
-        <v>27</v>
-      </c>
-      <c r="G11">
-        <v>0.75</v>
-      </c>
-      <c r="H11" t="s">
-        <v>22</v>
-      </c>
-      <c r="I11" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A12" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="B12" t="s">
-        <v>47</v>
-      </c>
-      <c r="C12" s="3">
-        <v>5</v>
-      </c>
-      <c r="D12" s="4">
-        <v>44417</v>
-      </c>
-      <c r="E12">
-        <v>900</v>
-      </c>
-      <c r="F12" t="s">
-        <v>27</v>
-      </c>
-      <c r="G12">
-        <v>0.75</v>
-      </c>
-      <c r="H12" t="s">
-        <v>22</v>
-      </c>
-      <c r="I12" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A13" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="B13" t="s">
-        <v>47</v>
-      </c>
-      <c r="C13" s="3">
-        <v>5</v>
-      </c>
-      <c r="D13" s="4">
-        <v>44417</v>
-      </c>
-      <c r="E13">
-        <v>900</v>
-      </c>
-      <c r="F13" t="s">
-        <v>27</v>
-      </c>
-      <c r="G13">
-        <v>0.75</v>
-      </c>
-      <c r="H13" t="s">
-        <v>22</v>
-      </c>
-      <c r="I13" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A14" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="B14" t="s">
-        <v>47</v>
-      </c>
-      <c r="C14" s="3">
-        <v>5</v>
-      </c>
-      <c r="D14" s="4">
-        <v>44417</v>
-      </c>
-      <c r="E14">
-        <v>900</v>
-      </c>
-      <c r="F14" t="s">
-        <v>27</v>
-      </c>
-      <c r="G14">
-        <v>0.75</v>
-      </c>
-      <c r="H14" t="s">
-        <v>22</v>
-      </c>
-      <c r="I14" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A15" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="B15" t="s">
-        <v>47</v>
-      </c>
-      <c r="C15" s="3">
-        <v>5</v>
-      </c>
-      <c r="D15" s="4">
-        <v>44417</v>
-      </c>
-      <c r="E15">
-        <v>900</v>
-      </c>
-      <c r="F15" t="s">
-        <v>27</v>
-      </c>
-      <c r="G15">
-        <v>0.75</v>
-      </c>
-      <c r="H15" t="s">
-        <v>22</v>
-      </c>
-      <c r="I15" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A16" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="B16" t="s">
-        <v>47</v>
-      </c>
-      <c r="C16" s="3">
-        <v>5</v>
-      </c>
-      <c r="D16" s="4">
-        <v>44417</v>
-      </c>
-      <c r="E16">
-        <v>900</v>
-      </c>
-      <c r="F16" t="s">
-        <v>27</v>
-      </c>
-      <c r="G16">
-        <v>0.75</v>
-      </c>
-      <c r="H16" t="s">
-        <v>22</v>
-      </c>
-      <c r="I16" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A17" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="B17" t="s">
-        <v>47</v>
-      </c>
-      <c r="C17" s="3">
-        <v>5</v>
-      </c>
-      <c r="D17" s="4">
-        <v>44417</v>
-      </c>
-      <c r="E17">
-        <v>900</v>
-      </c>
-      <c r="F17" t="s">
-        <v>27</v>
-      </c>
-      <c r="G17">
-        <v>0.75</v>
-      </c>
-      <c r="H17" t="s">
-        <v>22</v>
-      </c>
-      <c r="I17" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A18" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="B18" t="s">
-        <v>47</v>
-      </c>
-      <c r="C18" s="3">
-        <v>5</v>
-      </c>
-      <c r="D18" s="4">
-        <v>44417</v>
-      </c>
-      <c r="E18">
-        <v>900</v>
-      </c>
-      <c r="F18" t="s">
-        <v>27</v>
-      </c>
-      <c r="G18">
-        <v>0.75</v>
-      </c>
-      <c r="H18" t="s">
-        <v>22</v>
-      </c>
-      <c r="I18" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A19" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="B19" t="s">
-        <v>47</v>
-      </c>
-      <c r="C19" s="3">
-        <v>5</v>
-      </c>
-      <c r="D19" s="4">
-        <v>44417</v>
-      </c>
-      <c r="E19">
-        <v>900</v>
-      </c>
-      <c r="F19" t="s">
-        <v>27</v>
-      </c>
-      <c r="G19">
-        <v>0.75</v>
-      </c>
-      <c r="H19" t="s">
-        <v>22</v>
-      </c>
-      <c r="I19" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A20" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="B20" t="s">
-        <v>47</v>
-      </c>
-      <c r="C20" s="3">
-        <v>5</v>
-      </c>
-      <c r="D20" s="4">
-        <v>44417</v>
-      </c>
-      <c r="E20">
-        <v>900</v>
-      </c>
-      <c r="F20" t="s">
-        <v>27</v>
-      </c>
-      <c r="G20">
-        <v>0.75</v>
-      </c>
-      <c r="H20" t="s">
-        <v>22</v>
-      </c>
-      <c r="I20" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A21" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="B21" t="s">
-        <v>47</v>
-      </c>
-      <c r="C21" s="3">
-        <v>5</v>
-      </c>
-      <c r="D21" s="4">
-        <v>44417</v>
-      </c>
-      <c r="E21">
-        <v>900</v>
-      </c>
-      <c r="F21" t="s">
-        <v>27</v>
-      </c>
-      <c r="G21">
-        <v>0.75</v>
-      </c>
-      <c r="H21" t="s">
-        <v>22</v>
-      </c>
-      <c r="I21" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A22" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="B22" t="s">
-        <v>67</v>
-      </c>
-      <c r="C22" s="3">
-        <v>6</v>
-      </c>
-      <c r="D22" s="4">
-        <v>44414</v>
-      </c>
-      <c r="E22">
-        <v>690</v>
-      </c>
-      <c r="F22" t="s">
-        <v>18</v>
-      </c>
-      <c r="G22">
-        <v>2.02</v>
-      </c>
-      <c r="H22" t="s">
-        <v>22</v>
-      </c>
-      <c r="I22" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A23" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="B23" t="s">
-        <v>67</v>
-      </c>
-      <c r="C23" s="3">
-        <v>6</v>
-      </c>
-      <c r="D23" s="4">
-        <v>44414</v>
-      </c>
-      <c r="E23">
-        <v>690</v>
-      </c>
-      <c r="F23" t="s">
-        <v>18</v>
-      </c>
-      <c r="G23">
-        <v>2.02</v>
-      </c>
-      <c r="H23" t="s">
-        <v>22</v>
-      </c>
-      <c r="I23" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A24" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="B24" t="s">
-        <v>67</v>
-      </c>
-      <c r="C24" s="3">
-        <v>6</v>
-      </c>
-      <c r="D24" s="4">
-        <v>44414</v>
-      </c>
-      <c r="E24">
-        <v>690</v>
-      </c>
-      <c r="F24" t="s">
-        <v>18</v>
-      </c>
-      <c r="G24">
-        <v>2.02</v>
-      </c>
-      <c r="H24" t="s">
-        <v>22</v>
-      </c>
-      <c r="I24" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A25" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="B25" t="s">
-        <v>67</v>
-      </c>
-      <c r="C25" s="3">
-        <v>6</v>
-      </c>
-      <c r="D25" s="4">
-        <v>44414</v>
-      </c>
-      <c r="E25">
-        <v>690</v>
-      </c>
-      <c r="F25" t="s">
-        <v>18</v>
-      </c>
-      <c r="G25">
-        <v>2.02</v>
-      </c>
-      <c r="H25" t="s">
-        <v>22</v>
-      </c>
-      <c r="I25" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A26" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="B26" t="s">
-        <v>67</v>
-      </c>
-      <c r="C26" s="3">
-        <v>7</v>
-      </c>
-      <c r="D26" s="4">
-        <v>47839</v>
-      </c>
-      <c r="E26">
-        <v>340</v>
-      </c>
-      <c r="F26" t="s">
-        <v>18</v>
-      </c>
-      <c r="G26">
-        <v>1.123</v>
-      </c>
-      <c r="H26" t="s">
-        <v>22</v>
-      </c>
-      <c r="I26" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A27" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="B27" t="s">
-        <v>67</v>
-      </c>
-      <c r="C27" s="3">
-        <v>7</v>
-      </c>
-      <c r="D27" s="4">
-        <v>47839</v>
-      </c>
-      <c r="E27">
-        <v>340</v>
-      </c>
-      <c r="F27" t="s">
-        <v>18</v>
-      </c>
-      <c r="G27">
-        <v>1.123</v>
-      </c>
-      <c r="H27" t="s">
-        <v>22</v>
-      </c>
-      <c r="I27" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A28" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="B28" t="s">
-        <v>67</v>
-      </c>
-      <c r="C28" s="3">
-        <v>7</v>
-      </c>
-      <c r="D28" s="4">
-        <v>47839</v>
-      </c>
-      <c r="E28">
-        <v>340</v>
-      </c>
-      <c r="F28" t="s">
-        <v>18</v>
-      </c>
-      <c r="G28">
-        <v>1.123</v>
-      </c>
-      <c r="H28" t="s">
-        <v>22</v>
-      </c>
-      <c r="I28" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A29" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="B29" t="s">
-        <v>67</v>
-      </c>
-      <c r="C29" s="3">
-        <v>7</v>
-      </c>
-      <c r="D29" s="4">
-        <v>47839</v>
-      </c>
-      <c r="E29">
-        <v>340</v>
-      </c>
-      <c r="F29" t="s">
-        <v>18</v>
-      </c>
-      <c r="G29">
-        <v>1.123</v>
-      </c>
-      <c r="H29" t="s">
-        <v>22</v>
-      </c>
-      <c r="I29" t="s">
-        <v>64</v>
-      </c>
-    </row>
   </sheetData>
-  <autoFilter ref="A1:J29" xr:uid="{00000000-0001-0000-0100-000000000000}"/>
+  <autoFilter ref="A1:J8" xr:uid="{00000000-0001-0000-0100-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -1991,8 +1385,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:J29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A7" activeCellId="2" sqref="A3:XFD3 A5:XFD5 A7:XFD7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Get bonds by type and date
</commit_message>
<xml_diff>
--- a/utils/db-bonds-data.xlsx
+++ b/utils/db-bonds-data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DB\arrakis_v3\utils\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8470402-2994-4F48-B63B-5A7C9225F91F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90FD0180-CA10-4924-B809-3179F2FC6342}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1124,8 +1124,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:J8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>